<commit_message>
Correcciones de nombres de imágenes y de escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/Escaleta_CN_11_05_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion05/Escaleta_CN_11_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado11\guion05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Autor\Física\CN_11_05_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$31</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="215">
   <si>
     <t>Asignatura</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Evaluación</t>
   </si>
   <si>
-    <t>Banco de actividades: Fenómenos ondulatorios</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -494,54 +491,18 @@
     <t>Las ondas estacionarias en los instrumentos musicales</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las ondas en los intrumentos musicales</t>
-  </si>
-  <si>
-    <t>Las ondas, la música y la voz</t>
-  </si>
-  <si>
-    <t>Conoce las cualidades del sonido</t>
-  </si>
-  <si>
     <t>El sonido: naturaleza y propagación</t>
   </si>
   <si>
-    <t>Las ondas sonoras, la música y la voz</t>
-  </si>
-  <si>
-    <t>Interactivo para asociar los tipos de ondas estacionarias a instrumentos musicales determinados, y comprender su origen y propagación</t>
-  </si>
-  <si>
-    <t>Hacer una sección de ondas longitudinales, explicar cómo son cuando se habla de sonido (ilustrar el movimiento de resorte de las moléculas en el aire), y dar ejemplos concretos de instrumentos que producen este tipo de ondas. La segunda sección es similar, pero con ondas estacionarias transversales.</t>
-  </si>
-  <si>
-    <t>Actividad para analizar el tipo de ondas que producen los instrumentos musicales</t>
-  </si>
-  <si>
     <t>Actividad para analizar la formación y las características de las ondas estacionarias</t>
   </si>
   <si>
     <t>Preguntas de análisis sobre ondas estacionarias</t>
   </si>
   <si>
-    <t>Poner diferentes instrumentos para que se organicen en alguna de dos columnas: ondas transversales u ondas longitudinales</t>
-  </si>
-  <si>
-    <t>Actividad para clasificar instrumentos musicales en función del tipo de ondas que producen</t>
-  </si>
-  <si>
     <t>Hacer un texto que explique la formación de las ondas estacionarias a partir de la interferencia</t>
   </si>
   <si>
-    <t>Ondas estacionarias e interferencia</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer la relación entre la interferencia y las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Hacer preguntas acerca de diversos aspectos de las ondas estacionarias, su formación y sus características. Algunas pueden ser ejemplos de ondas, para determinar si son o no estacionarias.</t>
-  </si>
-  <si>
     <t>Recurso M2C-01</t>
   </si>
   <si>
@@ -551,95 +512,170 @@
     <t>Interactivo con vídeo que presenta las propiedades físicas del sonido y de sus correlatos acústicos</t>
   </si>
   <si>
-    <t>Actividad para reconocer las cualidades del sonido</t>
-  </si>
-  <si>
-    <t>Interactivo para comprender la música y la voz humana en términos de ondas</t>
-  </si>
-  <si>
-    <t>Hacer palabras o frases relacionadas con la música o la voz, y poner su descripción. Por ejemplo, tono, barítono, cuerdas vocales. Todo debe estar en términos de ondas.</t>
-  </si>
-  <si>
-    <t>Actividad para identificar el significado de diferentes términos acerca de la relación entre la música y la voz con las ondas sonoras</t>
+    <t>Recurso M11A-01</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema: Ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos acerca del tema: Ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Motor que incluye preguntas de respuesta abierta del tema Ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Recurso M102A-01</t>
+  </si>
+  <si>
+    <t>Preguntas de falso y verdadero sobre tipos de ondas e instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Actividad para identificar la veracidad de diversas afirmaciones sobre ondas estacionarias en instrumentos musicales</t>
+  </si>
+  <si>
+    <t>La naturaleza de la música</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar un experimento para generar una onda estacionaria con una cuerda</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las ondas en los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Competencias: formación de una onda estacionaria</t>
+  </si>
+  <si>
+    <t>Los sonidos musicales</t>
+  </si>
+  <si>
+    <t>El origen de las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Ondas estacionarias longitudinales y transversales</t>
+  </si>
+  <si>
+    <t>Los tipos de ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Actividad para comprender qué es la música en términos ondulatorios</t>
+  </si>
+  <si>
+    <t>Las cualidades del sonido</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer las principales características de las ondas sonoras</t>
+  </si>
+  <si>
+    <t>Recurso M2A-01</t>
+  </si>
+  <si>
+    <t>Hacer una sección explicándo qué es música, qué es ruido, y por qué las ondas estacionarias se relacionan con la música. Otra sección explica las carácterísticas del sonido altura, intensidad y timbre.</t>
+  </si>
+  <si>
+    <t>Hacer un texto acerca de las cualidades del sonido: altura, intensidad y timbre.</t>
+  </si>
+  <si>
+    <t>Describir diversos conceptos relacionados con la música, en términos de ondas.</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer y describir la música en términos de ondas sonoras</t>
+  </si>
+  <si>
+    <t>La música en términos de ondas</t>
+  </si>
+  <si>
+    <t>Música y ruido</t>
+  </si>
+  <si>
+    <t>Un contenedor es Música, y el otro es Ruido. Poner características que pertenezcan a uno u otro contenedor.</t>
+  </si>
+  <si>
+    <t>Actividad para diferenciar los sonidos musicales del ruido</t>
+  </si>
+  <si>
+    <t>Actividad para analizar la relación de la música con las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Preguntas de análisis sobre la relación entre las ondas estacionarias y la música</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Ondas estacionarias y música</t>
+  </si>
+  <si>
+    <t>Las ondas estacionarias y su relación con los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Interactivo para explicar el funcionamiento de los instrumentos musicales en términos de ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Hacer tres menús: instrumentos de cuerdas, instrumentos de viento, e instrumentos de percusión. Explicar la voz humana con los instrumentos de viento.</t>
+  </si>
+  <si>
+    <t>Los distintos tipos de instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Poner diferentes instrumentos para que se organicen en los contenedores viento, cuerdas o percusión</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer y clasificar algunas características de los distintos tipos de instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Recurso M10A-02</t>
+  </si>
+  <si>
+    <t>Ondas e instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Actividad para analizar el funcionamiento de los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Recurso M1C-01</t>
+  </si>
+  <si>
+    <t>Actividad para describir el funcionamiento de los instrumentos musicales en términos ondulatorios</t>
+  </si>
+  <si>
+    <t>La física de los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Hacer frases que describan las ondas en los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Hacer preguntas de análisis sobre ondas estacionarias en instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Describir como crear ondas estacionarias atando una cuerda a la pared y moviéndola con la mano. Cuando se logre, hay que medir amplitud, frecuencia , etc.</t>
+  </si>
+  <si>
+    <t>Los instrumentos de percusión</t>
+  </si>
+  <si>
+    <t>Hacer imágenes que muestren cosas relevantes de las ondas estacionarias, como un nodo, un antinodo, una onda reflejada, etc.</t>
+  </si>
+  <si>
+    <t>Los componentes de las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer distintos componentes de las ondas estacionarias a partir de su representación visual.</t>
+  </si>
+  <si>
+    <t>Recurso M3A-01</t>
+  </si>
+  <si>
+    <t>Hacer términos relacionados con ondas estacionarias y hacer su descripción</t>
   </si>
   <si>
     <t>Recurso M1B-01</t>
   </si>
   <si>
-    <t>Hacer una sección dedicada a la música, explicando la distribución de notas musicales, relacionándolas con su frecuencias correspondientes y recalcándo por qué un La de un violín se diferencia al de un piano. Diferenciar la música del ruido. La otra sección estudia la voz humana, explica e ilustra las cuerdas vocales y su funcionamiento, y clasifica los tipos de voz (soprano, barítono, etc.). Si no se puede aprovechar el video del sonido, explicar las cualidades del sonido en una sección más de este recurso. Que sea la primera de las tres.</t>
-  </si>
-  <si>
-    <t>Actividad para reforzar lo aprendido sobre la relación de la música y la voz con las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Describir diversas palabras relacionadas con la música o la voz, en términos de ondas</t>
-  </si>
-  <si>
-    <t>Recurso M11A-01</t>
-  </si>
-  <si>
-    <t>Las ondas sonoras</t>
-  </si>
-  <si>
-    <t>La música y la voz como ondas</t>
-  </si>
-  <si>
-    <t>Preguntas de análisis sobre ondas estacionarias en instrumentos musicales, tales como ¡Son todas las ondas sonoras ondas estacionarias?</t>
-  </si>
-  <si>
-    <t>La relación de las ondas estacionarias con la música y la voz humana</t>
-  </si>
-  <si>
-    <t>Mapa conceptual del tema: Ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Evalúa tus conocimientos acerca del tema: Ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema Ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Ondas, música y voz</t>
-  </si>
-  <si>
-    <t>Actividad para analizar la relación de la música y la voz con las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Preguntas de nálisis sobre ondas, música y voz</t>
-  </si>
-  <si>
-    <t>Preguntas de falso y verdadero sobre tipos de ondas e instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Actividad para identificar la veracidad de diversas afirmaciones sobre ondas estacionarias en instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Tipos de ondas estacionarias y su relación con los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Ondas estacionarias e instrumentos</t>
-  </si>
-  <si>
-    <t>La naturaleza de la música</t>
-  </si>
-  <si>
-    <t>Competencias: Formación de una onda estacionaria</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar un experimento para generar una onda estacionaria con una cuerda</t>
-  </si>
-  <si>
-    <t>Describir como crear ondas estacionarias atando una cuerda a la pared o moviéndola con la mano. Cuando se logre, hay que medir amplitud, frecuencia , etc.</t>
-  </si>
-  <si>
-    <t>Recurso M102AB-01</t>
+    <t>Banco de actividades: Ondas estacionarias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,6 +702,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -800,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -856,34 +899,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -924,6 +949,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,144 +1275,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U294"/>
+  <dimension ref="A1:U296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U5" sqref="U5:U6"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="45.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="30.265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.86328125" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.86328125" customWidth="1"/>
-    <col min="11" max="11" width="13.265625" customWidth="1"/>
-    <col min="12" max="12" width="17.3984375" customWidth="1"/>
-    <col min="13" max="14" width="9.265625" customWidth="1"/>
-    <col min="15" max="15" width="37.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.59765625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.06640625" customWidth="1"/>
-    <col min="19" max="19" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.73046875" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="43"/>
+      <c r="O1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="46" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+    <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="32"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="47"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D3" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="27"/>
       <c r="G3" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1375,7 +1421,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1388,7 +1434,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1397,35 +1443,37 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="S3" s="19" t="s">
-        <v>128</v>
-      </c>
       <c r="T3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D4" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="13"/>
+        <v>148</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1434,7 +1482,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1443,11 +1491,11 @@
         <v>8</v>
       </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="52" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1456,35 +1504,37 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S4" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="T4" s="12" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D5" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="25"/>
+        <v>148</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>176</v>
+      </c>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1493,7 +1543,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1503,10 +1553,10 @@
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1515,37 +1565,37 @@
         <v>6</v>
       </c>
       <c r="R5" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="S5" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="T5" s="21" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="U5" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D6" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>122</v>
+        <v>148</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>176</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>154</v>
+        <v>209</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1554,7 +1604,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1564,10 +1614,10 @@
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1576,44 +1626,46 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S6" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="T6" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="U6" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>211</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D7" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="25"/>
+        <v>148</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1621,12 +1673,12 @@
       <c r="L7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="O7" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -1635,57 +1687,57 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="U7" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>155</v>
+      <c r="D8" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="8"/>
       <c r="O8" s="9" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -1694,96 +1746,90 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="13"/>
+      <c r="D9" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="25"/>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>194</v>
-      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>122</v>
-      </c>
+      <c r="D10" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="13"/>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1792,7 +1838,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1802,10 +1848,10 @@
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1814,90 +1860,94 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S10" s="10" t="s">
+      <c r="T10" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="T10" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="U10" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D11" s="15" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
+      <c r="N11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>182</v>
+      </c>
       <c r="P11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="10" t="s">
-        <v>141</v>
+      <c r="Q11" s="10">
+        <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D12" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="25"/>
+        <v>173</v>
+      </c>
+      <c r="E12" s="13"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1906,75 +1956,81 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
+      <c r="N12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>183</v>
+      </c>
       <c r="P12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>141</v>
+        <v>20</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D13" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="13"/>
+        <v>173</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N13" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="O13" s="9" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -1983,44 +2039,44 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="13"/>
+      <c r="D14" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="25"/>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2028,12 +2084,12 @@
       <c r="L14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="M14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="8"/>
       <c r="O14" s="9" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>19</v>
@@ -2042,35 +2098,37 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="13"/>
+      <c r="D15" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>207</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2079,7 +2137,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2089,49 +2147,49 @@
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q15" s="10">
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S15" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S15" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="T15" s="12" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>157</v>
+      <c r="D16" s="26" t="s">
+        <v>154</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2140,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2150,10 +2208,10 @@
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2162,32 +2220,34 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S16" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="T16" s="12" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="13"/>
+      <c r="D17" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>207</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
         <v>199</v>
@@ -2199,57 +2259,59 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="10">
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S17" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="T17" s="12" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="13"/>
+      <c r="D18" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2258,7 +2320,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2267,34 +2329,48 @@
         <v>8</v>
       </c>
       <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="9"/>
+      <c r="N18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>205</v>
+      </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="10"/>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="Q18" s="10">
+        <v>6</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D19" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2303,7 +2379,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2313,9 +2389,11 @@
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O19" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2323,27 +2401,27 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S19" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="S19" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="T19" s="12" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>145</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>124</v>
@@ -2351,7 +2429,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2360,7 +2438,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2369,76 +2447,132 @@
         <v>8</v>
       </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="8" t="s">
-        <v>121</v>
-      </c>
+      <c r="N20" s="8"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="10">
-        <v>6</v>
-      </c>
-      <c r="R20" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="15"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="10"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="6"/>
+      <c r="G21" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="9">
+        <v>19</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
+      <c r="N21" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="10"/>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="15"/>
+      <c r="P21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>6</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T21" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="6"/>
+      <c r="G22" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" s="9">
+        <v>20</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="N22" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="10"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="P22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>6</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T22" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="U22" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="24"/>
       <c r="C23" s="25"/>
@@ -2461,7 +2595,7 @@
       <c r="T23" s="12"/>
       <c r="U23" s="10"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
@@ -2484,7 +2618,7 @@
       <c r="T24" s="12"/>
       <c r="U24" s="10"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25"/>
@@ -2507,7 +2641,7 @@
       <c r="T25" s="12"/>
       <c r="U25" s="10"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -2530,7 +2664,7 @@
       <c r="T26" s="12"/>
       <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
@@ -2553,7 +2687,7 @@
       <c r="T27" s="12"/>
       <c r="U27" s="10"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
@@ -2576,7 +2710,7 @@
       <c r="T28" s="12"/>
       <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
@@ -2599,10 +2733,10 @@
       <c r="T29" s="12"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="24"/>
-      <c r="C30" s="14"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="15"/>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
@@ -2622,10 +2756,10 @@
       <c r="T30" s="12"/>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="15"/>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
@@ -2645,7 +2779,7 @@
       <c r="T31" s="12"/>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="24"/>
       <c r="C32" s="14"/>
@@ -2668,7 +2802,7 @@
       <c r="T32" s="12"/>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="24"/>
       <c r="C33" s="14"/>
@@ -2691,7 +2825,7 @@
       <c r="T33" s="12"/>
       <c r="U33" s="10"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="24"/>
       <c r="C34" s="14"/>
@@ -2714,7 +2848,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="24"/>
       <c r="C35" s="14"/>
@@ -2737,7 +2871,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="24"/>
       <c r="C36" s="14"/>
@@ -2760,7 +2894,7 @@
       <c r="T36" s="12"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="24"/>
       <c r="C37" s="14"/>
@@ -2783,7 +2917,7 @@
       <c r="T37" s="12"/>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="24"/>
       <c r="C38" s="14"/>
@@ -2806,9 +2940,9 @@
       <c r="T38" s="12"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="14"/>
       <c r="D39" s="15"/>
       <c r="E39" s="13"/>
@@ -2829,9 +2963,9 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="14"/>
       <c r="D40" s="15"/>
       <c r="E40" s="13"/>
@@ -2852,7 +2986,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="10"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -2875,7 +3009,7 @@
       <c r="T41" s="12"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -2898,7 +3032,7 @@
       <c r="T42" s="12"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -2921,7 +3055,7 @@
       <c r="T43" s="12"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -2944,7 +3078,7 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -2967,7 +3101,7 @@
       <c r="T45" s="12"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -2990,7 +3124,7 @@
       <c r="T46" s="12"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -3013,7 +3147,7 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -3036,7 +3170,7 @@
       <c r="T48" s="12"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -3059,7 +3193,7 @@
       <c r="T49" s="12"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -3082,7 +3216,7 @@
       <c r="T50" s="12"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -3105,7 +3239,7 @@
       <c r="T51" s="12"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -3128,7 +3262,7 @@
       <c r="T52" s="12"/>
       <c r="U52" s="10"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -3151,7 +3285,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -3174,7 +3308,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="10"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -3197,7 +3331,7 @@
       <c r="T55" s="12"/>
       <c r="U55" s="10"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -3220,7 +3354,7 @@
       <c r="T56" s="12"/>
       <c r="U56" s="10"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -3243,7 +3377,7 @@
       <c r="T57" s="12"/>
       <c r="U57" s="10"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -3266,7 +3400,7 @@
       <c r="T58" s="12"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -3289,7 +3423,7 @@
       <c r="T59" s="12"/>
       <c r="U59" s="10"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -3312,7 +3446,7 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -3335,7 +3469,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="10"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -3358,7 +3492,7 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
@@ -3381,7 +3515,7 @@
       <c r="T63" s="12"/>
       <c r="U63" s="10"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
@@ -3404,7 +3538,7 @@
       <c r="T64" s="12"/>
       <c r="U64" s="10"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
@@ -3427,7 +3561,7 @@
       <c r="T65" s="12"/>
       <c r="U65" s="10"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -3450,7 +3584,7 @@
       <c r="T66" s="12"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
@@ -3473,7 +3607,7 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
@@ -3496,7 +3630,7 @@
       <c r="T68" s="12"/>
       <c r="U68" s="10"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
@@ -3519,7 +3653,7 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
@@ -3542,7 +3676,7 @@
       <c r="T70" s="12"/>
       <c r="U70" s="10"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14"/>
@@ -3565,7 +3699,7 @@
       <c r="T71" s="12"/>
       <c r="U71" s="10"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -3588,7 +3722,7 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14"/>
@@ -3611,7 +3745,7 @@
       <c r="T73" s="12"/>
       <c r="U73" s="10"/>
     </row>
-    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14"/>
@@ -3634,7 +3768,7 @@
       <c r="T74" s="12"/>
       <c r="U74" s="10"/>
     </row>
-    <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="13"/>
       <c r="C75" s="14"/>
@@ -3657,7 +3791,7 @@
       <c r="T75" s="12"/>
       <c r="U75" s="10"/>
     </row>
-    <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="13"/>
       <c r="C76" s="14"/>
@@ -3680,7 +3814,7 @@
       <c r="T76" s="12"/>
       <c r="U76" s="10"/>
     </row>
-    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="13"/>
       <c r="C77" s="14"/>
@@ -3703,7 +3837,7 @@
       <c r="T77" s="12"/>
       <c r="U77" s="10"/>
     </row>
-    <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="13"/>
       <c r="C78" s="14"/>
@@ -3726,7 +3860,7 @@
       <c r="T78" s="12"/>
       <c r="U78" s="10"/>
     </row>
-    <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="13"/>
       <c r="C79" s="14"/>
@@ -3749,7 +3883,7 @@
       <c r="T79" s="12"/>
       <c r="U79" s="10"/>
     </row>
-    <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="13"/>
       <c r="C80" s="14"/>
@@ -3772,372 +3906,424 @@
       <c r="T80" s="12"/>
       <c r="U80" s="10"/>
     </row>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
+    <row r="81" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="10"/>
+      <c r="R81" s="11"/>
+      <c r="S81" s="10"/>
+      <c r="T81" s="12"/>
+      <c r="U81" s="10"/>
+    </row>
+    <row r="82" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="17"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="10"/>
+      <c r="R82" s="11"/>
+      <c r="S82" s="10"/>
+      <c r="T82" s="12"/>
+      <c r="U82" s="10"/>
+    </row>
+    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A108" t="s">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A110" t="s">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A112" t="s">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A113" t="s">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A114" t="s">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A116" t="s">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A118" t="s">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A119" t="s">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A120" t="s">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A121" t="s">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A122" t="s">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A124" t="s">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A126" t="s">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A127" t="s">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A128" t="s">
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A129" t="s">
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A130" t="s">
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U29">
+  <autoFilter ref="A1:U31">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4152,12 +4338,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4168,31 +4348,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N80</xm:sqref>
+          <xm:sqref>N3:N82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A80</xm:sqref>
+          <xm:sqref>A3:A82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I80 P3:P80 K3:K80</xm:sqref>
+          <xm:sqref>K3:K82 P3:P82 I3:I82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L80</xm:sqref>
+          <xm:sqref>L3:L82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M80</xm:sqref>
+          <xm:sqref>M3:M82</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4208,27 +4388,27 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="2"/>
-    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="2"/>
+    <col min="13" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="24.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -4245,7 +4425,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -4269,7 +4449,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -4288,7 +4468,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4307,7 +4487,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4323,7 +4503,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4340,7 +4520,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -4357,7 +4537,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4372,7 +4552,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4387,7 +4567,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4402,7 +4582,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4417,7 +4597,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4432,7 +4612,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4447,7 +4627,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4462,7 +4642,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4477,7 +4657,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -4492,7 +4672,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -4506,7 +4686,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -4520,7 +4700,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -4534,7 +4714,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -4548,7 +4728,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -4563,7 +4743,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -4578,7 +4758,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -4593,7 +4773,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4608,7 +4788,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4623,7 +4803,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4638,7 +4818,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4653,7 +4833,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4668,7 +4848,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4683,7 +4863,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4698,7 +4878,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -4713,7 +4893,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -4728,7 +4908,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -4743,7 +4923,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4758,7 +4938,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4773,7 +4953,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4788,7 +4968,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4803,7 +4983,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4818,7 +4998,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -4833,7 +5013,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -4848,7 +5028,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -4863,7 +5043,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -4878,7 +5058,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -4893,7 +5073,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -4908,7 +5088,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -4923,7 +5103,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -4938,7 +5118,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -4953,7 +5133,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -4968,7 +5148,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -4980,7 +5160,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -4992,7 +5172,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -5005,7 +5185,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5018,7 +5198,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -5031,7 +5211,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5044,7 +5224,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -5057,7 +5237,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -5070,7 +5250,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -5083,7 +5263,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -5096,7 +5276,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -5109,7 +5289,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -5122,7 +5302,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -5135,7 +5315,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -5148,7 +5328,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -5161,7 +5341,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -5174,7 +5354,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -5187,7 +5367,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -5200,7 +5380,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -5213,7 +5393,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -5226,7 +5406,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -5239,7 +5419,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -5252,7 +5432,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -5266,7 +5446,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -5280,7 +5460,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -5294,7 +5474,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5308,7 +5488,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5322,7 +5502,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5336,7 +5516,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5350,7 +5530,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5364,7 +5544,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5378,7 +5558,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5392,7 +5572,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5406,7 +5586,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5420,7 +5600,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5434,7 +5614,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5448,7 +5628,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5462,7 +5642,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5476,7 +5656,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5490,7 +5670,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5504,7 +5684,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5518,7 +5698,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5532,7 +5712,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5546,7 +5726,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5560,7 +5740,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5574,7 +5754,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5588,7 +5768,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5602,7 +5782,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5616,7 +5796,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5630,7 +5810,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5644,7 +5824,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5658,7 +5838,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5672,7 +5852,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5686,7 +5866,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5700,7 +5880,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5714,7 +5894,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5728,7 +5908,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5742,7 +5922,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5756,7 +5936,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5770,7 +5950,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5784,7 +5964,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5798,7 +5978,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -5812,7 +5992,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5826,7 +6006,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -5840,7 +6020,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5854,7 +6034,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -5868,7 +6048,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5882,7 +6062,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -5896,7 +6076,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5910,7 +6090,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -5924,7 +6104,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -5938,7 +6118,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -5952,7 +6132,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -5966,7 +6146,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -5980,7 +6160,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -5994,7 +6174,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -6008,7 +6188,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6022,7 +6202,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -6036,7 +6216,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -6050,7 +6230,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -6064,7 +6244,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -6078,7 +6258,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -6092,7 +6272,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6106,7 +6286,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -6120,7 +6300,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>

<commit_message>
Actualización (0) de escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/Escaleta_CN_11_05_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion05/Escaleta_CN_11_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Autor\Física\CN_11_05_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado11\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$29</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="203">
   <si>
     <t>Asignatura</t>
   </si>
@@ -404,6 +404,9 @@
     <t>Evaluación</t>
   </si>
   <si>
+    <t>Banco de actividades: Fenómenos ondulatorios</t>
+  </si>
+  <si>
     <t>RF</t>
   </si>
   <si>
@@ -491,18 +494,54 @@
     <t>Las ondas estacionarias en los instrumentos musicales</t>
   </si>
   <si>
+    <t>Refuerza tu aprendizaje: Las ondas en los intrumentos musicales</t>
+  </si>
+  <si>
+    <t>Las ondas, la música y la voz</t>
+  </si>
+  <si>
+    <t>Conoce las cualidades del sonido</t>
+  </si>
+  <si>
     <t>El sonido: naturaleza y propagación</t>
   </si>
   <si>
+    <t>Las ondas sonoras, la música y la voz</t>
+  </si>
+  <si>
+    <t>Interactivo para asociar los tipos de ondas estacionarias a instrumentos musicales determinados, y comprender su origen y propagación</t>
+  </si>
+  <si>
+    <t>Hacer una sección de ondas longitudinales, explicar cómo son cuando se habla de sonido (ilustrar el movimiento de resorte de las moléculas en el aire), y dar ejemplos concretos de instrumentos que producen este tipo de ondas. La segunda sección es similar, pero con ondas estacionarias transversales.</t>
+  </si>
+  <si>
+    <t>Actividad para analizar el tipo de ondas que producen los instrumentos musicales</t>
+  </si>
+  <si>
     <t>Actividad para analizar la formación y las características de las ondas estacionarias</t>
   </si>
   <si>
     <t>Preguntas de análisis sobre ondas estacionarias</t>
   </si>
   <si>
+    <t>Poner diferentes instrumentos para que se organicen en alguna de dos columnas: ondas transversales u ondas longitudinales</t>
+  </si>
+  <si>
+    <t>Actividad para clasificar instrumentos musicales en función del tipo de ondas que producen</t>
+  </si>
+  <si>
     <t>Hacer un texto que explique la formación de las ondas estacionarias a partir de la interferencia</t>
   </si>
   <si>
+    <t>Ondas estacionarias e interferencia</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer la relación entre la interferencia y las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Hacer preguntas acerca de diversos aspectos de las ondas estacionarias, su formación y sus características. Algunas pueden ser ejemplos de ondas, para determinar si son o no estacionarias.</t>
+  </si>
+  <si>
     <t>Recurso M2C-01</t>
   </si>
   <si>
@@ -512,9 +551,45 @@
     <t>Interactivo con vídeo que presenta las propiedades físicas del sonido y de sus correlatos acústicos</t>
   </si>
   <si>
+    <t>Actividad para reconocer las cualidades del sonido</t>
+  </si>
+  <si>
+    <t>Interactivo para comprender la música y la voz humana en términos de ondas</t>
+  </si>
+  <si>
+    <t>Hacer palabras o frases relacionadas con la música o la voz, y poner su descripción. Por ejemplo, tono, barítono, cuerdas vocales. Todo debe estar en términos de ondas.</t>
+  </si>
+  <si>
+    <t>Actividad para identificar el significado de diferentes términos acerca de la relación entre la música y la voz con las ondas sonoras</t>
+  </si>
+  <si>
+    <t>Recurso M1B-01</t>
+  </si>
+  <si>
+    <t>Hacer una sección dedicada a la música, explicando la distribución de notas musicales, relacionándolas con su frecuencias correspondientes y recalcándo por qué un La de un violín se diferencia al de un piano. Diferenciar la música del ruido. La otra sección estudia la voz humana, explica e ilustra las cuerdas vocales y su funcionamiento, y clasifica los tipos de voz (soprano, barítono, etc.). Si no se puede aprovechar el video del sonido, explicar las cualidades del sonido en una sección más de este recurso. Que sea la primera de las tres.</t>
+  </si>
+  <si>
+    <t>Actividad para reforzar lo aprendido sobre la relación de la música y la voz con las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Describir diversas palabras relacionadas con la música o la voz, en términos de ondas</t>
+  </si>
+  <si>
     <t>Recurso M11A-01</t>
   </si>
   <si>
+    <t>Las ondas sonoras</t>
+  </si>
+  <si>
+    <t>La música y la voz como ondas</t>
+  </si>
+  <si>
+    <t>Preguntas de análisis sobre ondas estacionarias en instrumentos musicales, tales como ¡Son todas las ondas sonoras ondas estacionarias?</t>
+  </si>
+  <si>
+    <t>La relación de las ondas estacionarias con la música y la voz humana</t>
+  </si>
+  <si>
     <t>Mapa conceptual del tema: Ondas estacionarias</t>
   </si>
   <si>
@@ -524,7 +599,13 @@
     <t>Motor que incluye preguntas de respuesta abierta del tema Ondas estacionarias</t>
   </si>
   <si>
-    <t>Recurso M102A-01</t>
+    <t>Refuerza tu aprendizaje: Ondas, música y voz</t>
+  </si>
+  <si>
+    <t>Actividad para analizar la relación de la música y la voz con las ondas estacionarias</t>
+  </si>
+  <si>
+    <t>Preguntas de nálisis sobre ondas, música y voz</t>
   </si>
   <si>
     <t>Preguntas de falso y verdadero sobre tipos de ondas e instrumentos musicales</t>
@@ -533,149 +614,32 @@
     <t>Actividad para identificar la veracidad de diversas afirmaciones sobre ondas estacionarias en instrumentos musicales</t>
   </si>
   <si>
+    <t>Tipos de ondas estacionarias y su relación con los instrumentos musicales</t>
+  </si>
+  <si>
+    <t>Ondas estacionarias e instrumentos</t>
+  </si>
+  <si>
     <t>La naturaleza de la música</t>
   </si>
   <si>
+    <t>Competencias: Formación de una onda estacionaria</t>
+  </si>
+  <si>
     <t>Actividad que propone realizar un experimento para generar una onda estacionaria con una cuerda</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las ondas en los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Competencias: formación de una onda estacionaria</t>
-  </si>
-  <si>
-    <t>Los sonidos musicales</t>
-  </si>
-  <si>
-    <t>El origen de las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Ondas estacionarias longitudinales y transversales</t>
-  </si>
-  <si>
-    <t>Los tipos de ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Actividad para comprender qué es la música en términos ondulatorios</t>
-  </si>
-  <si>
-    <t>Las cualidades del sonido</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer las principales características de las ondas sonoras</t>
-  </si>
-  <si>
-    <t>Recurso M2A-01</t>
-  </si>
-  <si>
-    <t>Hacer una sección explicándo qué es música, qué es ruido, y por qué las ondas estacionarias se relacionan con la música. Otra sección explica las carácterísticas del sonido altura, intensidad y timbre.</t>
-  </si>
-  <si>
-    <t>Hacer un texto acerca de las cualidades del sonido: altura, intensidad y timbre.</t>
-  </si>
-  <si>
-    <t>Describir diversos conceptos relacionados con la música, en términos de ondas.</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer y describir la música en términos de ondas sonoras</t>
-  </si>
-  <si>
-    <t>La música en términos de ondas</t>
-  </si>
-  <si>
-    <t>Música y ruido</t>
-  </si>
-  <si>
-    <t>Un contenedor es Música, y el otro es Ruido. Poner características que pertenezcan a uno u otro contenedor.</t>
-  </si>
-  <si>
-    <t>Actividad para diferenciar los sonidos musicales del ruido</t>
-  </si>
-  <si>
-    <t>Actividad para analizar la relación de la música con las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Preguntas de análisis sobre la relación entre las ondas estacionarias y la música</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Ondas estacionarias y música</t>
-  </si>
-  <si>
-    <t>Las ondas estacionarias y su relación con los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Interactivo para explicar el funcionamiento de los instrumentos musicales en términos de ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Hacer tres menús: instrumentos de cuerdas, instrumentos de viento, e instrumentos de percusión. Explicar la voz humana con los instrumentos de viento.</t>
-  </si>
-  <si>
-    <t>Los distintos tipos de instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Poner diferentes instrumentos para que se organicen en los contenedores viento, cuerdas o percusión</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer y clasificar algunas características de los distintos tipos de instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Recurso M10A-02</t>
-  </si>
-  <si>
-    <t>Ondas e instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Actividad para analizar el funcionamiento de los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Recurso M1C-01</t>
-  </si>
-  <si>
-    <t>Actividad para describir el funcionamiento de los instrumentos musicales en términos ondulatorios</t>
-  </si>
-  <si>
-    <t>La física de los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Hacer frases que describan las ondas en los instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Hacer preguntas de análisis sobre ondas estacionarias en instrumentos musicales</t>
-  </si>
-  <si>
-    <t>Describir como crear ondas estacionarias atando una cuerda a la pared y moviéndola con la mano. Cuando se logre, hay que medir amplitud, frecuencia , etc.</t>
-  </si>
-  <si>
-    <t>Los instrumentos de percusión</t>
-  </si>
-  <si>
-    <t>Hacer imágenes que muestren cosas relevantes de las ondas estacionarias, como un nodo, un antinodo, una onda reflejada, etc.</t>
-  </si>
-  <si>
-    <t>Los componentes de las ondas estacionarias</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer distintos componentes de las ondas estacionarias a partir de su representación visual.</t>
-  </si>
-  <si>
-    <t>Recurso M3A-01</t>
-  </si>
-  <si>
-    <t>Hacer términos relacionados con ondas estacionarias y hacer su descripción</t>
-  </si>
-  <si>
-    <t>Recurso M1B-01</t>
-  </si>
-  <si>
-    <t>Banco de actividades: Ondas estacionarias</t>
+    <t>Describir como crear ondas estacionarias atando una cuerda a la pared o moviéndola con la mano. Cuando se logre, hay que medir amplitud, frecuencia , etc.</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,13 +666,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -843,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -899,16 +856,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,27 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,144 +1229,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U296"/>
+  <dimension ref="A1:U294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="U5" sqref="U5:U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.86328125" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.86328125" customWidth="1"/>
+    <col min="11" max="11" width="13.265625" customWidth="1"/>
+    <col min="12" max="12" width="17.3984375" customWidth="1"/>
+    <col min="13" max="14" width="9.265625" customWidth="1"/>
+    <col min="15" max="15" width="37.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.59765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.06640625" customWidth="1"/>
+    <col min="19" max="19" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="43"/>
-      <c r="O1" s="31" t="s">
+      <c r="N1" s="49"/>
+      <c r="O1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="38"/>
+    <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="42"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="44"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="47"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="32"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="27"/>
       <c r="G3" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1421,7 +1375,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1434,7 +1388,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1443,37 +1397,35 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>174</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1482,7 +1434,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1491,11 +1443,11 @@
         <v>8</v>
       </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1504,37 +1456,35 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>176</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E5" s="25"/>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1543,7 +1493,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1553,10 +1503,10 @@
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1565,37 +1515,37 @@
         <v>6</v>
       </c>
       <c r="R5" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S5" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="U5" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>176</v>
+        <v>149</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>209</v>
+        <v>154</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1604,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1614,10 +1564,10 @@
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1626,46 +1576,44 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="S6" s="10" t="s">
         <v>127</v>
       </c>
+      <c r="S6" s="19" t="s">
+        <v>133</v>
+      </c>
       <c r="T6" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>122</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E7" s="25"/>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1673,12 +1621,12 @@
       <c r="L7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="M7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8"/>
       <c r="O7" s="9" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -1687,57 +1635,57 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>173</v>
+        <v>146</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>155</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="O8" s="9" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -1746,90 +1694,96 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E9" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
+      <c r="N9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="P9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>140</v>
+        <v>20</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E10" s="13"/>
+        <v>146</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1838,7 +1792,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1848,10 +1802,10 @@
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1860,94 +1814,90 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>182</v>
-      </c>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="10">
-        <v>6</v>
+      <c r="Q11" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E12" s="13"/>
+        <v>160</v>
+      </c>
+      <c r="E12" s="25"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1956,81 +1906,75 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="8"/>
-      <c r="N12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>183</v>
-      </c>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>122</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="E13" s="13"/>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="8"/>
       <c r="O13" s="9" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2039,44 +1983,44 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="T13" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="U13" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="13"/>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2084,12 +2028,12 @@
       <c r="L14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="O14" s="9" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>19</v>
@@ -2098,37 +2042,35 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>207</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2137,7 +2079,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2147,49 +2089,49 @@
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="10">
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2198,7 +2140,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2208,10 +2150,10 @@
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2220,34 +2162,32 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>207</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
         <v>199</v>
@@ -2259,59 +2199,57 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17" s="10">
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>122</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="13"/>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>171</v>
+        <v>10</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2320,7 +2258,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2329,48 +2267,34 @@
         <v>8</v>
       </c>
       <c r="M18" s="8"/>
-      <c r="N18" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>205</v>
-      </c>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="10">
-        <v>6</v>
-      </c>
-      <c r="R18" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="U18" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q18" s="10"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2379,7 +2303,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2389,11 +2313,9 @@
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>206</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2401,27 +2323,27 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>124</v>
@@ -2429,7 +2351,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2438,7 +2360,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2447,132 +2369,76 @@
         <v>8</v>
       </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="N20" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="10"/>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>124</v>
-      </c>
+      <c r="Q20" s="10">
+        <v>6</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="H21" s="9">
-        <v>19</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="6"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="N21" s="8"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="10">
-        <v>6</v>
-      </c>
-      <c r="R21" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>124</v>
-      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="10"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="H22" s="9">
-        <v>20</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="6"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="N22" s="8"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="10">
-        <v>6</v>
-      </c>
-      <c r="R22" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="T22" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P22" s="9"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="10"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="4"/>
       <c r="B23" s="24"/>
       <c r="C23" s="25"/>
@@ -2595,7 +2461,7 @@
       <c r="T23" s="12"/>
       <c r="U23" s="10"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="4"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
@@ -2618,7 +2484,7 @@
       <c r="T24" s="12"/>
       <c r="U24" s="10"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="4"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25"/>
@@ -2641,7 +2507,7 @@
       <c r="T25" s="12"/>
       <c r="U25" s="10"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="4"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -2664,7 +2530,7 @@
       <c r="T26" s="12"/>
       <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="4"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
@@ -2687,7 +2553,7 @@
       <c r="T27" s="12"/>
       <c r="U27" s="10"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="4"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
@@ -2710,7 +2576,7 @@
       <c r="T28" s="12"/>
       <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="4"/>
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
@@ -2733,10 +2599,10 @@
       <c r="T29" s="12"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="4"/>
       <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="15"/>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
@@ -2756,10 +2622,10 @@
       <c r="T30" s="12"/>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="4"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="15"/>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
@@ -2779,7 +2645,7 @@
       <c r="T31" s="12"/>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A32" s="4"/>
       <c r="B32" s="24"/>
       <c r="C32" s="14"/>
@@ -2802,7 +2668,7 @@
       <c r="T32" s="12"/>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" s="4"/>
       <c r="B33" s="24"/>
       <c r="C33" s="14"/>
@@ -2825,7 +2691,7 @@
       <c r="T33" s="12"/>
       <c r="U33" s="10"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A34" s="4"/>
       <c r="B34" s="24"/>
       <c r="C34" s="14"/>
@@ -2848,7 +2714,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A35" s="4"/>
       <c r="B35" s="24"/>
       <c r="C35" s="14"/>
@@ -2871,7 +2737,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" s="4"/>
       <c r="B36" s="24"/>
       <c r="C36" s="14"/>
@@ -2894,7 +2760,7 @@
       <c r="T36" s="12"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" s="4"/>
       <c r="B37" s="24"/>
       <c r="C37" s="14"/>
@@ -2917,7 +2783,7 @@
       <c r="T37" s="12"/>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A38" s="4"/>
       <c r="B38" s="24"/>
       <c r="C38" s="14"/>
@@ -2940,9 +2806,9 @@
       <c r="T38" s="12"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A39" s="4"/>
-      <c r="B39" s="24"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="14"/>
       <c r="D39" s="15"/>
       <c r="E39" s="13"/>
@@ -2963,9 +2829,9 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A40" s="4"/>
-      <c r="B40" s="24"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="14"/>
       <c r="D40" s="15"/>
       <c r="E40" s="13"/>
@@ -2986,7 +2852,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="10"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -3009,7 +2875,7 @@
       <c r="T41" s="12"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -3032,7 +2898,7 @@
       <c r="T42" s="12"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -3055,7 +2921,7 @@
       <c r="T43" s="12"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -3078,7 +2944,7 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -3101,7 +2967,7 @@
       <c r="T45" s="12"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -3124,7 +2990,7 @@
       <c r="T46" s="12"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -3147,7 +3013,7 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -3170,7 +3036,7 @@
       <c r="T48" s="12"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -3193,7 +3059,7 @@
       <c r="T49" s="12"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -3216,7 +3082,7 @@
       <c r="T50" s="12"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -3239,7 +3105,7 @@
       <c r="T51" s="12"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -3262,7 +3128,7 @@
       <c r="T52" s="12"/>
       <c r="U52" s="10"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -3285,7 +3151,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -3308,7 +3174,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="10"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -3331,7 +3197,7 @@
       <c r="T55" s="12"/>
       <c r="U55" s="10"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -3354,7 +3220,7 @@
       <c r="T56" s="12"/>
       <c r="U56" s="10"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -3377,7 +3243,7 @@
       <c r="T57" s="12"/>
       <c r="U57" s="10"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -3400,7 +3266,7 @@
       <c r="T58" s="12"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -3423,7 +3289,7 @@
       <c r="T59" s="12"/>
       <c r="U59" s="10"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -3446,7 +3312,7 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -3469,7 +3335,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="10"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -3492,7 +3358,7 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
@@ -3515,7 +3381,7 @@
       <c r="T63" s="12"/>
       <c r="U63" s="10"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
@@ -3538,7 +3404,7 @@
       <c r="T64" s="12"/>
       <c r="U64" s="10"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
@@ -3561,7 +3427,7 @@
       <c r="T65" s="12"/>
       <c r="U65" s="10"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -3584,7 +3450,7 @@
       <c r="T66" s="12"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
@@ -3607,7 +3473,7 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A68" s="4"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
@@ -3630,7 +3496,7 @@
       <c r="T68" s="12"/>
       <c r="U68" s="10"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A69" s="4"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
@@ -3653,7 +3519,7 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A70" s="4"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
@@ -3676,7 +3542,7 @@
       <c r="T70" s="12"/>
       <c r="U70" s="10"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="4"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14"/>
@@ -3699,7 +3565,7 @@
       <c r="T71" s="12"/>
       <c r="U71" s="10"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="4"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -3722,7 +3588,7 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="4"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14"/>
@@ -3745,7 +3611,7 @@
       <c r="T73" s="12"/>
       <c r="U73" s="10"/>
     </row>
-    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="4"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14"/>
@@ -3768,7 +3634,7 @@
       <c r="T74" s="12"/>
       <c r="U74" s="10"/>
     </row>
-    <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="4"/>
       <c r="B75" s="13"/>
       <c r="C75" s="14"/>
@@ -3791,7 +3657,7 @@
       <c r="T75" s="12"/>
       <c r="U75" s="10"/>
     </row>
-    <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="4"/>
       <c r="B76" s="13"/>
       <c r="C76" s="14"/>
@@ -3814,7 +3680,7 @@
       <c r="T76" s="12"/>
       <c r="U76" s="10"/>
     </row>
-    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="4"/>
       <c r="B77" s="13"/>
       <c r="C77" s="14"/>
@@ -3837,7 +3703,7 @@
       <c r="T77" s="12"/>
       <c r="U77" s="10"/>
     </row>
-    <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A78" s="4"/>
       <c r="B78" s="13"/>
       <c r="C78" s="14"/>
@@ -3860,7 +3726,7 @@
       <c r="T78" s="12"/>
       <c r="U78" s="10"/>
     </row>
-    <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="4"/>
       <c r="B79" s="13"/>
       <c r="C79" s="14"/>
@@ -3883,7 +3749,7 @@
       <c r="T79" s="12"/>
       <c r="U79" s="10"/>
     </row>
-    <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A80" s="4"/>
       <c r="B80" s="13"/>
       <c r="C80" s="14"/>
@@ -3906,424 +3772,372 @@
       <c r="T80" s="12"/>
       <c r="U80" s="10"/>
     </row>
-    <row r="81" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="8"/>
-      <c r="O81" s="9"/>
-      <c r="P81" s="9"/>
-      <c r="Q81" s="10"/>
-      <c r="R81" s="11"/>
-      <c r="S81" s="10"/>
-      <c r="T81" s="12"/>
-      <c r="U81" s="10"/>
-    </row>
-    <row r="82" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="6"/>
-      <c r="M82" s="8"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="9"/>
-      <c r="P82" s="9"/>
-      <c r="Q82" s="10"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="10"/>
-      <c r="T82" s="12"/>
-      <c r="U82" s="10"/>
-    </row>
-    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="293" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="294" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <autoFilter ref="A1:U31">
+  <autoFilter ref="A1:U29">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4338,6 +4152,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4348,31 +4168,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N82</xm:sqref>
+          <xm:sqref>N3:N80</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A82</xm:sqref>
+          <xm:sqref>A3:A80</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K82 P3:P82 I3:I82</xm:sqref>
+          <xm:sqref>I3:I80 P3:P80 K3:K80</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L82</xm:sqref>
+          <xm:sqref>L3:L80</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M82</xm:sqref>
+          <xm:sqref>M3:M80</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4388,27 +4208,27 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="2"/>
-    <col min="14" max="14" width="24.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
+    <col min="13" max="13" width="11.3984375" style="2"/>
+    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -4425,7 +4245,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -4449,7 +4269,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -4468,7 +4288,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4487,7 +4307,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4503,7 +4323,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4520,7 +4340,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -4537,7 +4357,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4552,7 +4372,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4567,7 +4387,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4582,7 +4402,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4597,7 +4417,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4612,7 +4432,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4627,7 +4447,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4642,7 +4462,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4657,7 +4477,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -4672,7 +4492,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -4686,7 +4506,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -4700,7 +4520,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -4714,7 +4534,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -4728,7 +4548,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -4743,7 +4563,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -4758,7 +4578,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -4773,7 +4593,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4788,7 +4608,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4803,7 +4623,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4818,7 +4638,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4833,7 +4653,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4848,7 +4668,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4863,7 +4683,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4878,7 +4698,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -4893,7 +4713,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -4908,7 +4728,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -4923,7 +4743,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4938,7 +4758,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4953,7 +4773,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4968,7 +4788,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4983,7 +4803,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4998,7 +4818,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -5013,7 +4833,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5028,7 +4848,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -5043,7 +4863,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -5058,7 +4878,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -5073,7 +4893,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -5088,7 +4908,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -5103,7 +4923,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -5118,7 +4938,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5133,7 +4953,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -5148,7 +4968,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -5160,7 +4980,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -5172,7 +4992,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -5185,7 +5005,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5198,7 +5018,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -5211,7 +5031,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5224,7 +5044,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -5237,7 +5057,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -5250,7 +5070,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -5263,7 +5083,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -5276,7 +5096,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -5289,7 +5109,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -5302,7 +5122,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -5315,7 +5135,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -5328,7 +5148,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -5341,7 +5161,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -5354,7 +5174,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -5367,7 +5187,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -5380,7 +5200,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -5393,7 +5213,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -5406,7 +5226,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -5419,7 +5239,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -5432,7 +5252,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -5446,7 +5266,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -5460,7 +5280,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -5474,7 +5294,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5488,7 +5308,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5502,7 +5322,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5516,7 +5336,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5530,7 +5350,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5544,7 +5364,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5558,7 +5378,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5572,7 +5392,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5586,7 +5406,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5600,7 +5420,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5614,7 +5434,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5628,7 +5448,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5642,7 +5462,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5656,7 +5476,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5670,7 +5490,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5684,7 +5504,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5698,7 +5518,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5712,7 +5532,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5726,7 +5546,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5740,7 +5560,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5754,7 +5574,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5768,7 +5588,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5782,7 +5602,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5796,7 +5616,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5810,7 +5630,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5824,7 +5644,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5838,7 +5658,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5852,7 +5672,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5866,7 +5686,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5880,7 +5700,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5894,7 +5714,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5908,7 +5728,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5922,7 +5742,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5936,7 +5756,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5950,7 +5770,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5964,7 +5784,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5978,7 +5798,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -5992,7 +5812,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -6006,7 +5826,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -6020,7 +5840,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6034,7 +5854,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -6048,7 +5868,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -6062,7 +5882,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -6076,7 +5896,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -6090,7 +5910,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -6104,7 +5924,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -6118,7 +5938,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -6132,7 +5952,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6146,7 +5966,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -6160,7 +5980,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -6174,7 +5994,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -6188,7 +6008,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6202,7 +6022,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -6216,7 +6036,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -6230,7 +6050,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -6244,7 +6064,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -6258,7 +6078,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -6272,7 +6092,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6286,7 +6106,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -6300,7 +6120,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>